<commit_message>
Update and add test and bug report Excel files
- Updated API Test Cases and Full Test Cases Report Excel documents.
- Added a new Grad Project Bug Report Excel file to the Documents directory.
</commit_message>
<xml_diff>
--- a/Documents/API Test Cases for (Automation Exercise).xlsx
+++ b/Documents/API Test Cases for (Automation Exercise).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="425">
   <si>
     <t>ID</t>
   </si>
@@ -695,409 +695,409 @@
     <t>{"responseCode":200,"products":[...]}</t>
   </si>
   <si>
+    <t>Ali Ashour</t>
+  </si>
+  <si>
+    <t>TC_API01_002</t>
+  </si>
+  <si>
+    <t>Verify response structure</t>
+  </si>
+  <si>
+    <t>Response matches expected JSON schema</t>
+  </si>
+  <si>
+    <t>TC_API01_003</t>
+  </si>
+  <si>
+    <t>Verify request without authentication works</t>
+  </si>
+  <si>
+    <t>Response code=200 and data returned successfully</t>
+  </si>
+  <si>
+    <t>TC_API01_004</t>
+  </si>
+  <si>
+    <t>Verify response time</t>
+  </si>
+  <si>
+    <t>Response time ≤ 2 seconds</t>
+  </si>
+  <si>
+    <t>TC_API01_005</t>
+  </si>
+  <si>
+    <t>Verify invalid method returns error</t>
+  </si>
+  <si>
+    <t>POST/PUT</t>
+  </si>
+  <si>
+    <t>{"responseCode":405,"message":"This request method is not supported."}</t>
+  </si>
+  <si>
+    <t>TC_API04_001</t>
+  </si>
+  <si>
+    <t>Verify PUT method not supported</t>
+  </si>
+  <si>
+    <t>/api/brandsList</t>
+  </si>
+  <si>
+    <t>TC_API04_002</t>
+  </si>
+  <si>
+    <t>Verify GET method works for same endpoint</t>
+  </si>
+  <si>
+    <t>{"responseCode":200,"brands":[...]}</t>
+  </si>
+  <si>
+    <t>TC_API04_003</t>
+  </si>
+  <si>
+    <t>Verify invalid URL returns error</t>
+  </si>
+  <si>
+    <t>/api/brandsListt</t>
+  </si>
+  <si>
+    <t>{"responseCode":404,"message":"Not Found"}</t>
+  </si>
+  <si>
+    <t>TC_API05_001</t>
+  </si>
+  <si>
+    <t>Verify successful search with valid keyword</t>
+  </si>
+  <si>
+    <t>/api/searchProduct</t>
+  </si>
+  <si>
+    <t>{"search_product":"top"}</t>
+  </si>
+  <si>
+    <t>TC_API05_002</t>
+  </si>
+  <si>
+    <t>Verify search with invalid keyword</t>
+  </si>
+  <si>
+    <t>{"search_product":"randomword"}</t>
+  </si>
+  <si>
+    <t>{"responseCode":200,"products":[]}</t>
+  </si>
+  <si>
+    <t>TC_API05_003</t>
+  </si>
+  <si>
+    <t>Verify search parameter is mandatory</t>
+  </si>
+  <si>
+    <t>{"responseCode":400,"message":"Bad request, search_product parameter is missing"}</t>
+  </si>
+  <si>
+    <t>TC_API05_004</t>
+  </si>
+  <si>
+    <t>Verify case-insensitivity of search</t>
+  </si>
+  <si>
+    <t>{"search_product":"Top"}</t>
+  </si>
+  <si>
+    <t>Response same as lowercase search</t>
+  </si>
+  <si>
+    <t>TC_API05_005</t>
+  </si>
+  <si>
+    <t>Verify invalid method not allowed</t>
+  </si>
+  <si>
+    <t>TC_API05_006</t>
+  </si>
+  <si>
+    <t>TC_API05_007</t>
+  </si>
+  <si>
+    <t>Verify search_product field accepts only string</t>
+  </si>
+  <si>
+    <t>{"search_product":123}</t>
+  </si>
+  <si>
+    <t>{"responseCode":400,"message":"Invalid data type"}</t>
+  </si>
+  <si>
+    <t>TC_API05_008</t>
+  </si>
+  <si>
+    <t>Verify search_product cannot be empty string</t>
+  </si>
+  <si>
+    <t>{"search_product":""}</t>
+  </si>
+  <si>
+    <t>{"responseCode":400,"message":"search_product cannot be empty"}</t>
+  </si>
+  <si>
+    <t>TC_API05_009</t>
+  </si>
+  <si>
+    <t>Verify search_product with special characters</t>
+  </si>
+  <si>
+    <t>{"search_product":"@#$%"}</t>
+  </si>
+  <si>
+    <t>TC_API05_010</t>
+  </si>
+  <si>
+    <t>Verify maximum length of search_product</t>
+  </si>
+  <si>
+    <t>{"search_product":"&lt;255+ characters&gt;"}</t>
+  </si>
+  <si>
+    <t>{"responseCode":400,"message":"Input too long"}</t>
+  </si>
+  <si>
+    <t>TC_API05_011</t>
+  </si>
+  <si>
+    <t>Verify null value handling</t>
+  </si>
+  <si>
+    <t>{"search_product":null}</t>
+  </si>
+  <si>
+    <t>TC_API07_001</t>
+  </si>
+  <si>
+    <t>Verify login with valid email and password</t>
+  </si>
+  <si>
+    <t>{ "email":"Nxxx@gmail.com" , "password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>Nourhan Alabgar</t>
+  </si>
+  <si>
+    <t>TC_API07_002</t>
+  </si>
+  <si>
+    <t>Verify login is case-sensitive for email</t>
+  </si>
+  <si>
+    <t>{ "email": "NXXX@gmail.com", "password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API07_003</t>
+  </si>
+  <si>
+    <t>TC_API07_004</t>
+  </si>
+  <si>
+    <t>Verify login with extra name parameter</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxx@gmail.com", "password": "Nxxx@1234", "name":"Nxxx" }</t>
+  </si>
+  <si>
+    <t>TC_API10_001</t>
+  </si>
+  <si>
+    <t>Verify login with unauthenticated (invalid) email and password</t>
+  </si>
+  <si>
+    <t>{ "email":"Nxxxx@gmail.com" , "password": "Nxxxx@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API10_002</t>
+  </si>
+  <si>
+    <t>Verify login without email &amp; password</t>
+  </si>
+  <si>
+    <t>TC_API10_003</t>
+  </si>
+  <si>
+    <t>{"password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API10_004</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxx@gmail.com"}</t>
+  </si>
+  <si>
+    <t>TC_API10_005</t>
+  </si>
+  <si>
+    <t>Verify login with valid email and invalid password</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxx@gmail.com", "password": "12345" }</t>
+  </si>
+  <si>
+    <t>TC_API10_006</t>
+  </si>
+  <si>
+    <t>Verify login with invalid email and valid password</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxxx@gmail.com", "password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API10_007</t>
+  </si>
+  <si>
+    <t>Verify login with empty password</t>
+  </si>
+  <si>
+    <t>{ "email": "", "password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API10_008</t>
+  </si>
+  <si>
+    <t>Verify login with empty email</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxx@gmail.com", "password": "" }</t>
+  </si>
+  <si>
+    <t>TC_API10_009</t>
+  </si>
+  <si>
+    <t>Verify login with valid email and mismatched password</t>
+  </si>
+  <si>
+    <t>{ "email": "NxxxM@gmail.com", "password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API10_010</t>
+  </si>
+  <si>
+    <t>Verify login is case-sensitive for password</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxx@gmail.com", "password": "nXXX@1234" }</t>
+  </si>
+  <si>
+    <t>{"responseCode": 404, "message": "User not found!"}}</t>
+  </si>
+  <si>
+    <t>TC_API10_011</t>
+  </si>
+  <si>
+    <t>Verify login with name parameter instead of email</t>
+  </si>
+  <si>
+    <t>{ "name": "Nxxx", "password": "Nxxx@1234" }</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>TC_API14_001</t>
+  </si>
+  <si>
+    <t>Verify GET user account details by valid email</t>
+  </si>
+  <si>
+    <t>/api/getUserDetailByEmail</t>
+  </si>
+  <si>
+    <t>{ "email":"Nxxx@gmail.com"}</t>
+  </si>
+  <si>
+    <t>{"responseCode": 200, "user": {"id": 1076982, "name": "Nxxx", "email": "Nxxx@gmail.com", "title": "Miss", "birth_day": "14", "birth_month": "9", "birth_year": "2002", "first_name": "Nxxx", "last_name": "Axxxx", "company": "OpenAi", "address1": "Cairo", "address2": "Cairo", "country": "Egypt", "state": "Cairo", "city": "Cairo", "zipcode": "00000"}}</t>
+  </si>
+  <si>
+    <t>TC_API14_002</t>
+  </si>
+  <si>
+    <t>Verify GET user account details by invalid email</t>
+  </si>
+  <si>
+    <t>{ "email":"Nxxxx@gmail.com"}</t>
+  </si>
+  <si>
+    <t>{"responseCode": 404, "message": "Account not found with this email, try another email!"}</t>
+  </si>
+  <si>
+    <t>TC_API14_003</t>
+  </si>
+  <si>
+    <t>Verify GET login without email parameter</t>
+  </si>
+  <si>
+    <t>{"responseCode": 400, "message": "Bad request, email parameter is missing in GET request."}</t>
+  </si>
+  <si>
+    <t>TC_API14_004</t>
+  </si>
+  <si>
+    <t>Verify GET login without email value</t>
+  </si>
+  <si>
+    <t>{ "email": ""}</t>
+  </si>
+  <si>
+    <t>{"responseCode": 400, "message": "Bad request, email parameter is invalid"}</t>
+  </si>
+  <si>
+    <t>TC_API14_005</t>
+  </si>
+  <si>
+    <t>Verify GET login with invalid email format</t>
+  </si>
+  <si>
+    <t>{ "email": "Nxxx@gmail" }</t>
+  </si>
+  <si>
+    <t>TC_API14_006</t>
+  </si>
+  <si>
+    <t>Verify GET login is case-sensitive for email</t>
+  </si>
+  <si>
+    <t>{ "email": "NXXX@gmail.com"}</t>
+  </si>
+  <si>
+    <t>TC_API14_007</t>
+  </si>
+  <si>
+    <t>Verify GET login with name instead of email parameter</t>
+  </si>
+  <si>
+    <t>{ "name":"Nxxx"}</t>
+  </si>
+  <si>
+    <t>TC_API14_008</t>
+  </si>
+  <si>
+    <t>Verify login with POST method instead of GET (should not be accepted).</t>
+  </si>
+  <si>
+    <t>TC_API03_001</t>
+  </si>
+  <si>
+    <t>Verify GET returns all brand names successfully</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Response Code 200, list of brands returned</t>
+  </si>
+  <si>
     <t>NotTested</t>
-  </si>
-  <si>
-    <t>Ali Ashour</t>
-  </si>
-  <si>
-    <t>TC_API01_002</t>
-  </si>
-  <si>
-    <t>Verify response structure</t>
-  </si>
-  <si>
-    <t>Response matches expected JSON schema</t>
-  </si>
-  <si>
-    <t>TC_API01_003</t>
-  </si>
-  <si>
-    <t>Verify request without authentication works</t>
-  </si>
-  <si>
-    <t>Response code=200 and data returned successfully</t>
-  </si>
-  <si>
-    <t>TC_API01_004</t>
-  </si>
-  <si>
-    <t>Verify response time</t>
-  </si>
-  <si>
-    <t>Response time ≤ 2 seconds</t>
-  </si>
-  <si>
-    <t>TC_API01_005</t>
-  </si>
-  <si>
-    <t>Verify invalid method returns error</t>
-  </si>
-  <si>
-    <t>POST/PUT</t>
-  </si>
-  <si>
-    <t>{"responseCode":405,"message":"This request method is not supported."}</t>
-  </si>
-  <si>
-    <t>TC_API04_001</t>
-  </si>
-  <si>
-    <t>Verify PUT method not supported</t>
-  </si>
-  <si>
-    <t>/api/brandsList</t>
-  </si>
-  <si>
-    <t>TC_API04_002</t>
-  </si>
-  <si>
-    <t>Verify GET method works for same endpoint</t>
-  </si>
-  <si>
-    <t>{"responseCode":200,"brands":[...]}</t>
-  </si>
-  <si>
-    <t>TC_API04_003</t>
-  </si>
-  <si>
-    <t>Verify invalid URL returns error</t>
-  </si>
-  <si>
-    <t>/api/brandsListt</t>
-  </si>
-  <si>
-    <t>{"responseCode":404,"message":"Not Found"}</t>
-  </si>
-  <si>
-    <t>TC_API05_001</t>
-  </si>
-  <si>
-    <t>Verify successful search with valid keyword</t>
-  </si>
-  <si>
-    <t>/api/searchProduct</t>
-  </si>
-  <si>
-    <t>{"search_product":"top"}</t>
-  </si>
-  <si>
-    <t>TC_API05_002</t>
-  </si>
-  <si>
-    <t>Verify search with invalid keyword</t>
-  </si>
-  <si>
-    <t>{"search_product":"randomword"}</t>
-  </si>
-  <si>
-    <t>{"responseCode":200,"products":[]}</t>
-  </si>
-  <si>
-    <t>TC_API05_003</t>
-  </si>
-  <si>
-    <t>Verify search parameter is mandatory</t>
-  </si>
-  <si>
-    <t>{"responseCode":400,"message":"Bad request, search_product parameter is missing"}</t>
-  </si>
-  <si>
-    <t>TC_API05_004</t>
-  </si>
-  <si>
-    <t>Verify case-insensitivity of search</t>
-  </si>
-  <si>
-    <t>{"search_product":"Top"}</t>
-  </si>
-  <si>
-    <t>Response same as lowercase search</t>
-  </si>
-  <si>
-    <t>TC_API05_005</t>
-  </si>
-  <si>
-    <t>Verify invalid method not allowed</t>
-  </si>
-  <si>
-    <t>TC_API05_006</t>
-  </si>
-  <si>
-    <t>TC_API05_007</t>
-  </si>
-  <si>
-    <t>Verify search_product field accepts only string</t>
-  </si>
-  <si>
-    <t>{"search_product":123}</t>
-  </si>
-  <si>
-    <t>{"responseCode":400,"message":"Invalid data type"}</t>
-  </si>
-  <si>
-    <t>TC_API05_008</t>
-  </si>
-  <si>
-    <t>Verify search_product cannot be empty string</t>
-  </si>
-  <si>
-    <t>{"search_product":""}</t>
-  </si>
-  <si>
-    <t>{"responseCode":400,"message":"search_product cannot be empty"}</t>
-  </si>
-  <si>
-    <t>TC_API05_009</t>
-  </si>
-  <si>
-    <t>Verify search_product with special characters</t>
-  </si>
-  <si>
-    <t>{"search_product":"@#$%"}</t>
-  </si>
-  <si>
-    <t>TC_API05_010</t>
-  </si>
-  <si>
-    <t>Verify maximum length of search_product</t>
-  </si>
-  <si>
-    <t>{"search_product":"&lt;255+ characters&gt;"}</t>
-  </si>
-  <si>
-    <t>{"responseCode":400,"message":"Input too long"}</t>
-  </si>
-  <si>
-    <t>TC_API05_011</t>
-  </si>
-  <si>
-    <t>Verify null value handling</t>
-  </si>
-  <si>
-    <t>{"search_product":null}</t>
-  </si>
-  <si>
-    <t>TC_API07_001</t>
-  </si>
-  <si>
-    <t>Verify login with valid email and password</t>
-  </si>
-  <si>
-    <t>{ "email":"Nxxx@gmail.com" , "password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>Nourhan Alabgar</t>
-  </si>
-  <si>
-    <t>TC_API07_002</t>
-  </si>
-  <si>
-    <t>Verify login is case-sensitive for email</t>
-  </si>
-  <si>
-    <t>{ "email": "NXXX@gmail.com", "password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>TC_API07_003</t>
-  </si>
-  <si>
-    <t>TC_API07_004</t>
-  </si>
-  <si>
-    <t>Verify login with extra name parameter</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxx@gmail.com", "password": "Nxxx@1234", "name":"Nxxx" }</t>
-  </si>
-  <si>
-    <t>TC_API10_001</t>
-  </si>
-  <si>
-    <t>Verify login with unauthenticated (invalid) email and password</t>
-  </si>
-  <si>
-    <t>{ "email":"Nxxxx@gmail.com" , "password": "Nxxxx@1234" }</t>
-  </si>
-  <si>
-    <t>TC_API10_002</t>
-  </si>
-  <si>
-    <t>Verify login without email &amp; password</t>
-  </si>
-  <si>
-    <t>TC_API10_003</t>
-  </si>
-  <si>
-    <t>{"password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>TC_API10_004</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxx@gmail.com"}</t>
-  </si>
-  <si>
-    <t>TC_API10_005</t>
-  </si>
-  <si>
-    <t>Verify login with valid email and invalid password</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxx@gmail.com", "password": "12345" }</t>
-  </si>
-  <si>
-    <t>TC_API10_006</t>
-  </si>
-  <si>
-    <t>Verify login with invalid email and valid password</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxxx@gmail.com", "password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>TC_API10_007</t>
-  </si>
-  <si>
-    <t>Verify login with empty password</t>
-  </si>
-  <si>
-    <t>{ "email": "", "password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>TC_API10_008</t>
-  </si>
-  <si>
-    <t>Verify login with empty email</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxx@gmail.com", "password": "" }</t>
-  </si>
-  <si>
-    <t>TC_API10_009</t>
-  </si>
-  <si>
-    <t>Verify login with valid email and mismatched password</t>
-  </si>
-  <si>
-    <t>{ "email": "NxxxM@gmail.com", "password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>TC_API10_010</t>
-  </si>
-  <si>
-    <t>Verify login is case-sensitive for password</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxx@gmail.com", "password": "nXXX@1234" }</t>
-  </si>
-  <si>
-    <t>{"responseCode": 404, "message": "User not found!"}}</t>
-  </si>
-  <si>
-    <t>TC_API10_011</t>
-  </si>
-  <si>
-    <t>Verify login with name parameter instead of email</t>
-  </si>
-  <si>
-    <t>{ "name": "Nxxx", "password": "Nxxx@1234" }</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>TC_API14_001</t>
-  </si>
-  <si>
-    <t>Verify GET user account details by valid email</t>
-  </si>
-  <si>
-    <t>/api/getUserDetailByEmail</t>
-  </si>
-  <si>
-    <t>{ "email":"Nxxx@gmail.com"}</t>
-  </si>
-  <si>
-    <t>{"responseCode": 200, "user": {"id": 1076982, "name": "Nxxx", "email": "Nxxx@gmail.com", "title": "Miss", "birth_day": "14", "birth_month": "9", "birth_year": "2002", "first_name": "Nxxx", "last_name": "Axxxx", "company": "OpenAi", "address1": "Cairo", "address2": "Cairo", "country": "Egypt", "state": "Cairo", "city": "Cairo", "zipcode": "00000"}}</t>
-  </si>
-  <si>
-    <t>TC_API14_002</t>
-  </si>
-  <si>
-    <t>Verify GET user account details by invalid email</t>
-  </si>
-  <si>
-    <t>{ "email":"Nxxxx@gmail.com"}</t>
-  </si>
-  <si>
-    <t>{"responseCode": 404, "message": "Account not found with this email, try another email!"}</t>
-  </si>
-  <si>
-    <t>TC_API14_003</t>
-  </si>
-  <si>
-    <t>Verify GET login without email parameter</t>
-  </si>
-  <si>
-    <t>{"responseCode": 400, "message": "Bad request, email parameter is missing in GET request."}</t>
-  </si>
-  <si>
-    <t>TC_API14_004</t>
-  </si>
-  <si>
-    <t>Verify GET login without email value</t>
-  </si>
-  <si>
-    <t>{ "email": ""}</t>
-  </si>
-  <si>
-    <t>{"responseCode": 400, "message": "Bad request, email parameter is invalid"}</t>
-  </si>
-  <si>
-    <t>TC_API14_005</t>
-  </si>
-  <si>
-    <t>Verify GET login with invalid email format</t>
-  </si>
-  <si>
-    <t>{ "email": "Nxxx@gmail" }</t>
-  </si>
-  <si>
-    <t>TC_API14_006</t>
-  </si>
-  <si>
-    <t>Verify GET login is case-sensitive for email</t>
-  </si>
-  <si>
-    <t>{ "email": "NXXX@gmail.com"}</t>
-  </si>
-  <si>
-    <t>TC_API14_007</t>
-  </si>
-  <si>
-    <t>Verify GET login with name instead of email parameter</t>
-  </si>
-  <si>
-    <t>{ "name":"Nxxx"}</t>
-  </si>
-  <si>
-    <t>TC_API14_008</t>
-  </si>
-  <si>
-    <t>Verify login with POST method instead of GET (should not be accepted).</t>
-  </si>
-  <si>
-    <t>TC_API03_001</t>
-  </si>
-  <si>
-    <t>Verify GET returns all brand names successfully</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Response Code 200, list of brands returned</t>
   </si>
   <si>
     <t>Mooaz Elsayed</t>
@@ -1498,9 +1498,6 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1548,6 +1545,9 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1836,7 +1836,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A3:K8" displayName="API08_LoginWithoutEmail_Table_2" name="API08_LoginWithoutEmail_Table_2" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A3:K8" displayName="API01_LoginWithoutEmail_Table_2" name="API01_LoginWithoutEmail_Table_2" id="4">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Test Scenario" id="2"/>
@@ -7106,26 +7106,28 @@
       <c r="F4" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="12" t="s">
-        <v>213</v>
+      <c r="G4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>211</v>
@@ -7135,28 +7137,30 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="12" t="s">
-        <v>213</v>
+        <v>216</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>219</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>211</v>
@@ -7166,28 +7170,30 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="12" t="s">
-        <v>213</v>
+        <v>219</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>211</v>
@@ -7197,51 +7203,55 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="12" t="s">
-        <v>213</v>
+        <v>222</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>225</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>211</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="12" t="s">
-        <v>213</v>
+        <v>226</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9">
@@ -7287,95 +7297,101 @@
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>230</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="G12" s="13"/>
+        <v>226</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="H12" s="6" t="s">
-        <v>213</v>
+        <v>18</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="G13" s="13"/>
+        <v>232</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="H13" s="6" t="s">
-        <v>213</v>
+        <v>18</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="G14" s="13"/>
+        <v>236</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="H14" s="6" t="s">
-        <v>213</v>
+        <v>18</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -7421,79 +7437,83 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="12" t="s">
-        <v>213</v>
+      <c r="G18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="12" t="s">
-        <v>213</v>
+      <c r="G19" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" ht="22.5" customHeight="1">
       <c r="A20" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>247</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>14</v>
@@ -7502,282 +7522,300 @@
         <v>26</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="12" t="s">
-        <v>213</v>
+        <v>247</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="12" t="s">
-        <v>213</v>
+      <c r="G21" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>60</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="12" t="s">
-        <v>213</v>
+        <v>226</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>60</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="12" t="s">
-        <v>213</v>
+        <v>222</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>257</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="12" t="s">
-        <v>213</v>
+      <c r="G24" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>261</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="12" t="s">
-        <v>213</v>
+      <c r="G25" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>265</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="12" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>60</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>268</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="12" t="s">
-        <v>213</v>
+      <c r="G27" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="12" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>31</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -10630,7 +10668,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14"/>
+      <c r="A1" s="13"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
@@ -10670,10 +10708,10 @@
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>275</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -10682,7 +10720,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>45</v>
@@ -10697,18 +10735,18 @@
         <v>19</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -10717,7 +10755,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>45</v>
@@ -10732,15 +10770,15 @@
         <v>38</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
@@ -10767,18 +10805,18 @@
         <v>38</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>283</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -10787,7 +10825,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>45</v>
@@ -10802,46 +10840,46 @@
         <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>286</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -10850,7 +10888,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>30</v>
@@ -10865,18 +10903,18 @@
         <v>19</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>288</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>289</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -10900,15 +10938,15 @@
         <v>19</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -10920,7 +10958,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>16</v>
@@ -10935,15 +10973,15 @@
         <v>31</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>22</v>
@@ -10955,7 +10993,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>16</v>
@@ -10970,18 +11008,18 @@
         <v>31</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>13</v>
@@ -10990,7 +11028,7 @@
         <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>30</v>
@@ -11005,18 +11043,18 @@
         <v>38</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>13</v>
@@ -11025,7 +11063,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>30</v>
@@ -11040,18 +11078,18 @@
         <v>19</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>300</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>301</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>13</v>
@@ -11060,7 +11098,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>30</v>
@@ -11075,18 +11113,18 @@
         <v>19</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>303</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>304</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>13</v>
@@ -11095,7 +11133,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>30</v>
@@ -11110,18 +11148,18 @@
         <v>19</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>306</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>307</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>13</v>
@@ -11130,7 +11168,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>30</v>
@@ -11145,18 +11183,18 @@
         <v>19</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>309</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>310</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
@@ -11165,13 +11203,13 @@
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>18</v>
@@ -11180,18 +11218,18 @@
         <v>38</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" ht="22.5" customHeight="1">
       <c r="A18" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>313</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>314</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>13</v>
@@ -11200,7 +11238,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>16</v>
@@ -11215,14 +11253,14 @@
         <v>19</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" ht="22.5" customHeight="1">
@@ -11239,7 +11277,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>5</v>
@@ -11262,25 +11300,25 @@
     </row>
     <row r="25" ht="22.5" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="G25" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>18</v>
@@ -11289,33 +11327,33 @@
         <v>19</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" ht="22.5" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>323</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E26" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>18</v>
@@ -11324,21 +11362,21 @@
         <v>19</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" ht="22.5" customHeight="1">
       <c r="A27" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>327</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>53</v>
@@ -11347,10 +11385,10 @@
         <v>26</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>18</v>
@@ -11359,33 +11397,33 @@
         <v>19</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" ht="22.5" customHeight="1">
       <c r="A28" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>330</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>332</v>
-      </c>
       <c r="G28" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>18</v>
@@ -11394,33 +11432,33 @@
         <v>31</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" ht="22.5" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>334</v>
-      </c>
       <c r="C29" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>50</v>
@@ -11429,33 +11467,33 @@
         <v>38</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" ht="22.5" customHeight="1">
       <c r="A30" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>337</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>50</v>
@@ -11464,56 +11502,56 @@
         <v>19</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" ht="22.5" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>340</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>328</v>
+        <v>340</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>327</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="23" t="s">
+      <c r="I31" s="22" t="s">
         <v>31</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" ht="22.5" customHeight="1">
       <c r="A32" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>343</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>14</v>
@@ -11534,10 +11572,10 @@
         <v>38</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -11587,7 +11625,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14"/>
+      <c r="A1" s="13"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
@@ -11627,26 +11665,26 @@
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>345</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>31</v>
@@ -11666,20 +11704,20 @@
         <v>350</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>351</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>31</v>
@@ -11699,20 +11737,20 @@
         <v>353</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>354</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>31</v>
@@ -11725,32 +11763,32 @@
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
@@ -11766,14 +11804,14 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>357</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>31</v>
@@ -11799,14 +11837,14 @@
         <v>53</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>360</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>31</v>
@@ -11832,14 +11870,14 @@
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>364</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>38</v>
@@ -11865,7 +11903,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>5</v>
@@ -11900,14 +11938,14 @@
         <v>368</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>369</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>31</v>
@@ -11940,7 +11978,7 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>38</v>
@@ -11966,14 +12004,14 @@
         <v>368</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>364</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="6" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>38</v>
@@ -11994,7 +12032,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="7"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="25"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="3"/>
       <c r="K17" s="7"/>
     </row>
@@ -12007,20 +12045,20 @@
       <c r="F18" s="3"/>
       <c r="G18" s="7"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="25"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="3"/>
       <c r="K18" s="7"/>
     </row>
     <row r="19" ht="22.5" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="3"/>
       <c r="D19" s="5"/>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
       <c r="G19" s="7"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="25"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="3"/>
       <c r="K19" s="7"/>
     </row>
@@ -12030,12 +12068,12 @@
       <c r="C20" s="3"/>
       <c r="D20" s="5"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="22"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="7"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="23"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="26"/>
+      <c r="K20" s="25"/>
     </row>
     <row r="21" ht="22.5" customHeight="1">
       <c r="A21" s="3"/>
@@ -12139,7 +12177,7 @@
       <c r="B4" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>378</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -12153,7 +12191,7 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="12" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
@@ -12172,7 +12210,7 @@
       <c r="B5" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>385</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -12184,11 +12222,11 @@
       <c r="F5" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>55</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>19</v>
@@ -12207,7 +12245,7 @@
       <c r="B6" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>391</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -12223,7 +12261,7 @@
         <v>393</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>31</v>
@@ -12242,7 +12280,7 @@
       <c r="B7" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>391</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -12251,14 +12289,14 @@
       <c r="E7" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="30" t="s">
         <v>396</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>396</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>31</v>
@@ -12330,9 +12368,9 @@
       <c r="F11" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>19</v>
@@ -12363,9 +12401,9 @@
       <c r="F12" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>31</v>
@@ -12396,9 +12434,9 @@
       <c r="F13" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>38</v>
@@ -12429,9 +12467,9 @@
       <c r="F14" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="31"/>
       <c r="H14" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>19</v>
@@ -12462,9 +12500,9 @@
       <c r="F15" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="G15" s="13"/>
+      <c r="G15" s="31"/>
       <c r="H15" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>19</v>
@@ -12495,9 +12533,9 @@
       <c r="F16" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="G16" s="31"/>
       <c r="H16" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>31</v>
@@ -12528,9 +12566,9 @@
       <c r="F17" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="31"/>
       <c r="H17" s="32" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>31</v>
@@ -12848,7 +12886,7 @@
       </c>
       <c r="G113" s="35"/>
       <c r="H113" s="36" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="I113" s="35" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Reuploding documents in case of any changes
</commit_message>
<xml_diff>
--- a/Documents/API Test Cases for (Automation Exercise).xlsx
+++ b/Documents/API Test Cases for (Automation Exercise).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="433">
   <si>
     <t>ID</t>
   </si>
@@ -1097,7 +1097,7 @@
     <t>Response Code 200, list of brands returned</t>
   </si>
   <si>
-    <t>NotTested</t>
+    <t>{ "responseCode": 200, "brands": [ { "id": 1, "brand": "Polo" }, { "id": 2, "brand": "H&amp;M" }, { "id": 3, "brand": "Madame" }, { "id": 4, "brand": "Madame" }, { "id": 5, "brand": "Mast &amp; Harbour" }, { "id": 6, "brand": "H&amp;M" }, { "id": 7, "brand": "Madame" }, { "id": 8, "brand": "Polo" }, { "id": 11, "brand": "Babyhug" }, { "id": 12, "brand": "Babyhug" }, { "id": 13, "brand": "Allen Solly Junior" }, { "id": 14, "brand": "Kookie Kids" }, { "id": 15, "brand": "Babyhug" }, { "id": 16, "brand": "Babyhug" }, { "id": 18, "brand": "Kookie Kids" }, { "id": 19, "brand": "Allen Solly Junior" }, { "id": 20, "brand": "Kookie Kids" }, { "id": 21, "brand": "Biba" }, { "id": 22, "brand": "Biba" }, { "id": 23, "brand": "Biba" }, { "id": 24, "brand": "Allen Solly Junior" }, { "id": 28, "brand": "H&amp;M" }, { "id": 29, "brand": "Polo" }, { "id": 30, "brand": "Polo" }, { "id": 31, "brand": "H&amp;M" }, { "id": 33, "brand": "Polo" }, { "id": 35, "brand": "H&amp;M" }, { "id": 37, "brand": "Polo" }, { "id": 38, "brand": "Madame" }, { "id": 39, "brand": "Biba" }, { "id": 40, "brand": "Biba" }, { "id": 41, "brand": "Madame" }, { "id": 42, "brand": "Mast &amp; Harbour" }, { "id": 43, "brand": "Mast &amp; Harbour" } ] }</t>
   </si>
   <si>
     <t>Mooaz Elsayed</t>
@@ -1109,9 +1109,15 @@
     <t>Verify API returns error for invalid endpoint</t>
   </si>
   <si>
+    <t>/api/brandsListXYZ</t>
+  </si>
+  <si>
     <t>Response Code 404 Not Found</t>
   </si>
   <si>
+    <t>&lt;!DOCTYPE html&gt; &lt;html lang="en"&gt; &lt;head&gt; &lt;meta http-equiv="content-type" content="text/html; charset=utf-8"&gt; &lt;title&gt;Page not found at /api/brandsListXYZ &lt;/title&gt; &lt;meta name="robots" content="NONE,NOARCHIVE"&gt; &lt;style type="text/css"&gt; html * { padding: 0; margin: 0; } body * { padding: 10px 20px; } body * * { padding: 0; } body { font:small sans-serif; background:#eee; color:#000; } body&gt;div { border-bottom: 1px solid #ddd; } h1 { font-weight:normal; margin-bottom:.4em; } h1 span { font-size: 60%; color:#666; font-weight:normal; } table { border:none; border-collapse: collapse; width: 100%; } td, th { vertical-align:top; padding: 2px 3px; } th { width:12em; text-align:right; color:#666; padding-right:.5em; } #info { background:#f6f6f6; } #info ol { margin: 0.5em 4em; } #info ol li { font-family: monospace; } #summary { background: #ffc; } #explanation { background:#eee; border-bottom: 0px none; } pre.exception_value { font-family: sans-serif; color: #575757; font-size: 1.5em; margin: 10px 0 10px 0; } &lt;/style&gt; &lt;/head&gt; &lt;body&gt; &lt;div id="summary"&gt; &lt;h1&gt;Page not found &lt;span&gt;(404)&lt;/span&gt;&lt;/h1&gt; &lt;table class="meta"&gt; &lt;tr&gt; &lt;th&gt;Request Method:&lt;/th&gt; &lt;td&gt;GET&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;th&gt;Request URL:&lt;/th&gt; &lt;td&gt;https: //automationexercise.com/api/brandsListXYZ%0A&lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div id="info"&gt; &lt;p&gt; Using the URLconf defined in &lt;code&gt;automation_exercise.urls&lt;/code&gt;, Django tried these URL patterns, in this order: &lt;/p&gt; &lt;ol&gt; &lt;li&gt; admin/ &lt;/li&gt; &lt;li&gt; &lt;/li&gt; &lt;li&gt; get_product_picture/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; product_details/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; products &lt;/li&gt; &lt;li&gt; contact_us &lt;/li&gt; &lt;li&gt; add_to_cart/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; view_cart &lt;/li&gt; &lt;li&gt; delete_cart/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; login &lt;/li&gt; &lt;li&gt; signup &lt;/li&gt; &lt;li&gt; account_created &lt;/li&gt; &lt;li&gt; logout &lt;/li&gt; &lt;li&gt; checkout &lt;/li&gt; &lt;li&gt; payment &lt;/li&gt; &lt;li&gt; delete_account &lt;/li&gt; &lt;li&gt; brand_products/&amp;lt;str:brand&amp;gt; &lt;/li&gt; &lt;li&gt; category_products/&amp;lt;int:category_id&amp;gt; &lt;/li&gt; &lt;li&gt; test_cases &lt;/li&gt; &lt;li&gt; api_list &lt;/li&gt; &lt;li&gt; download_invoice/&amp;lt;int:overall_amount&amp;gt; &lt;/li&gt; &lt;li&gt; payment_done/&amp;lt;int:overall_amount&amp;gt; &lt;/li&gt; &lt;li&gt; video_tutorials &lt;/li&gt; &lt;li&gt; api/productsList &lt;/li&gt; &lt;li&gt; api/brandsList &lt;/li&gt; &lt;li&gt; api/searchProduct &lt;/li&gt; &lt;li&gt; api/verifyLogin &lt;/li&gt; &lt;li&gt; api/createAccount &lt;/li&gt; &lt;li&gt; api/deleteAccount &lt;/li&gt; &lt;li&gt; api/updateAccount &lt;/li&gt; &lt;li&gt; api/getUserDetailByEmail &lt;/li&gt; &lt;li&gt; &amp;lt;str:random_string&amp;gt; &lt;/li&gt; &lt;li&gt; ^static/(?P&amp;lt;path&amp;gt;.*)$ &lt;/li&gt; &lt;/ol&gt; &lt;p&gt; The current path, &lt;code&gt;api/brandsListXYZ &lt;/code&gt;, didn’t match any of these. &lt;/p&gt; &lt;/div&gt; &lt;div id="explanation"&gt; &lt;p&gt; You’re seeing this error because you have &lt;code&gt;DEBUG = True&lt;/code&gt; in your Django settings file. Change that to &lt;code&gt;False&lt;/code&gt;, and Django will display a standard 404 page. &lt;/p&gt; &lt;/div&gt; &lt;/body&gt; &lt;/html&gt;</t>
+  </si>
+  <si>
     <t>TC_API03_003</t>
   </si>
   <si>
@@ -1121,6 +1127,9 @@
     <t>Response Code 405 Method Not Allowed</t>
   </si>
   <si>
+    <t>{ "responseCode": 405, "message": "This request method is not supported." }</t>
+  </si>
+  <si>
     <t>TC_API02_001</t>
   </si>
   <si>
@@ -1139,6 +1148,9 @@
     <t>200 OK, list of products displayed</t>
   </si>
   <si>
+    <t>{ "responseCode": 200, "products": [ { "id": 1, "name": "Blue Top", "price": "Rs. 500", "brand": "Polo", "category": { "usertype": { "usertype": "Women" }, "category": "Tops" } }, { "id": 2, "name": "Men Tshirt", "price": "Rs. 400", "brand": "H&amp;M", "category": { "usertype": { "usertype": "Men" }, "category": "Tshirts" } }, { "id": 3, "name": "Sleeveless Dress", "price": "Rs. 1000", "brand": "Madame", "category": { "usertype": { "usertype": "Women" }, "category": "Dress" } }, { "id": 4, "name": "Stylish Dress", "price": "Rs. 1500", "brand": "Madame", "category": { "usertype": { "usertype": "Women" }, "category": "Dress" } }, { "id": 5, "name": "Winter Top", "price": "Rs. 600", "brand": "Mast &amp; Harbour", "category": { "usertype": { "usertype": "Women" }, "category": "Tops" } }, { "id": 6, "name": "Summer White Top", "price": "Rs. 400", "brand": "H&amp;M", "category": { "usertype": { "usertype": "Women" }, "category": "Tops" } }, { "id": 7, "name": "Madame Top For Women", "price": "Rs. 1000", "brand": "Madame", "category": { "usertype": { "usertype": "Women" }, "category": "Tops" } }, { "id": 8, "name": "Fancy Green Top", "price": "Rs. 700", "brand": "Polo", "category": { "usertype": { "usertype": "Women" }, "category": "Tops" } }, { "id": 11, "name": "Sleeves Printed Top - White", "price": "Rs. 499", "brand": "Babyhug", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 12, "name": "Half Sleeves Top Schiffli Detailing - Pink", "price": "Rs. 359", "brand": "Babyhug", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 13, "name": "Frozen Tops For Kids", "price": "Rs. 278", "brand": "Allen Solly Junior", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 14, "name": "Full Sleeves Top Cherry - Pink", "price": "Rs. 679", "brand": "Kookie Kids", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 15, "name": "Printed Off Shoulder Top - White", "price": "Rs. 315", "brand": "Babyhug", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 16, "name": "Sleeves Top and Short - Blue &amp; Pink", "price": "Rs. 478", "brand": "Babyhug", "category": { "usertype": { "usertype": "Kids" }, "category": "Dress" } }, { "id": 18, "name": "Little Girls Mr. Panda Shirt", "price": "Rs. 1200", "brand": "Kookie Kids", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 19, "name": "Sleeveless Unicorn Patch Gown - Pink", "price": "Rs. 1050", "brand": "Allen Solly Junior", "category": { "usertype": { "usertype": "Kids" }, "category": "Dress" } }, { "id": 20, "name": "Cotton Mull Embroidered Dress", "price": "Rs. 1190", "brand": "Kookie Kids", "category": { "usertype": { "usertype": "Kids" }, "category": "Dress" } }, { "id": 21, "name": "Blue Cotton Indie Mickey Dress", "price": "Rs. 1530", "brand": "Biba", "category": { "usertype": { "usertype": "Kids" }, "category": "Dress" } }, { "id": 22, "name": "Long Maxi Tulle Fancy Dress Up Outfits -Pink", "price": "Rs. 1600", "brand": "Biba", "category": { "usertype": { "usertype": "Kids" }, "category": "Dress" } }, { "id": 23, "name": "Sleeveless Unicorn Print Fit &amp; Flare Net Dress - Multi", "price": "Rs. 1100", "brand": "Biba", "category": { "usertype": { "usertype": "Kids" }, "category": "Dress" } }, { "id": 24, "name": "Colour Blocked Shirt – Sky Blue", "price": "Rs. 849", "brand": "Allen Solly Junior", "category": { "usertype": { "usertype": "Kids" }, "category": "Tops &amp; Shirts" } }, { "id": 28, "name": "Pure Cotton V-Neck T-Shirt", "price": "Rs. 1299", "brand": "H&amp;M", "category": { "usertype": { "usertype": "Men" }, "category": "Tshirts" } }, { "id": 29, "name": "Green Side Placket Detail T-Shirt", "price": "Rs. 1000", "brand": "Polo", "category": { "usertype": { "usertype": "Men" }, "category": "Tshirts" } }, { "id": 30, "name": "Premium Polo T-Shirts", "price": "Rs. 1500", "brand": "Polo", "category": { "usertype": { "usertype": "Men" }, "category": "Tshirts" } }, { "id": 31, "name": "Pure Cotton Neon Green Tshirt", "price": "Rs. 850", "brand": "H&amp;M", "category": { "usertype": { "usertype": "Men" }, "category": "Tshirts" } }, { "id": 33, "name": "Soft Stretch Jeans", "price": "Rs. 799", "brand": "Polo", "category": { "usertype": { "usertype": "Men" }, "category": "Jeans" } }, { "id": 35, "name": "Regular Fit Straight Jeans", "price": "Rs. 1200", "brand": "H&amp;M", "category": { "usertype": { "usertype": "Men" }, "category": "Jeans" } }, { "id": 37, "name": "Grunt Blue Slim Fit Jeans", "price": "Rs. 1400", "brand": "Polo", "category": { "usertype": { "usertype": "Men" }, "category": "Jeans" } }, { "id": 38, "name": "Rose Pink Embroidered Maxi Dress", "price": "Rs. 2300", "brand": "Madame", "category": { "usertype": { "usertype": "Women" }, "category": "Dress" } }, { "id": 39, "name": "Cotton Silk Hand Block Print Saree", "price": "Rs. 3000", "brand": "Biba", "category": { "usertype": { "usertype": "Women" }, "category": "Saree" } }, { "id": 40, "name": "Rust Red Linen Saree", "price": "Rs. 3500", "brand": "Biba", "category": { "usertype": { "usertype": "Women" }, "category": "Saree" } }, { "id": 41, "name": "Beautiful Peacock Blue Cotton Linen Saree", "price": "Rs. 5000", "brand": "Madame", "category": { "usertype": { "usertype": "Women" }, "category": "Saree" } }, { "id": 42, "name": "Lace Top For Women", "price": "Rs. 1400", "brand": "Mast &amp; Harbour", "category": { "usertype": { "usertype": "Women" }, "category": "Tops" } }, { "id": 43, "name": "GRAPHIC DESIGN MEN T SHIRT - BLUE", "price": "Rs. 1389", "brand": "Mast &amp; Harbour", "category": { "usertype": { "usertype": "Men" }, "category": "Tshirts" } } ] }</t>
+  </si>
+  <si>
     <t>TC_API02_003</t>
   </si>
   <si>
@@ -1151,6 +1163,9 @@
     <t>404 Not Found</t>
   </si>
   <si>
+    <t>&lt;!DOCTYPE html&gt; &lt;html lang="en"&gt; &lt;head&gt; &lt;meta http-equiv="content-type" content="text/html; charset=utf-8"&gt; &lt;title&gt;Page not found at /api/productList&lt;/title&gt; &lt;meta name="robots" content="NONE,NOARCHIVE"&gt; &lt;style type="text/css"&gt; html * { padding: 0; margin: 0; } body * { padding: 10px 20px; } body * * { padding: 0; } body { font:small sans-serif; background:#eee; color:#000; } body&gt;div { border-bottom: 1px solid #ddd; } h1 { font-weight:normal; margin-bottom:.4em; } h1 span { font-size: 60%; color:#666; font-weight:normal; } table { border:none; border-collapse: collapse; width: 100%; } td, th { vertical-align:top; padding: 2px 3px; } th { width:12em; text-align:right; color:#666; padding-right:.5em; } #info { background:#f6f6f6; } #info ol { margin: 0.5em 4em; } #info ol li { font-family: monospace; } #summary { background: #ffc; } #explanation { background:#eee; border-bottom: 0px none; } pre.exception_value { font-family: sans-serif; color: #575757; font-size: 1.5em; margin: 10px 0 10px 0; } &lt;/style&gt; &lt;/head&gt; &lt;body&gt; &lt;div id="summary"&gt; &lt;h1&gt;Page not found &lt;span&gt;(404)&lt;/span&gt;&lt;/h1&gt; &lt;table class="meta"&gt; &lt;tr&gt; &lt;th&gt;Request Method:&lt;/th&gt; &lt;td&gt;POST&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;th&gt;Request URL:&lt;/th&gt; &lt;td&gt;https: //automationexercise.com/api/productList&lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div id="info"&gt; &lt;p&gt; Using the URLconf defined in &lt;code&gt;automation_exercise.urls&lt;/code&gt;, Django tried these URL patterns, in this order: &lt;/p&gt; &lt;ol&gt; &lt;li&gt; admin/ &lt;/li&gt; &lt;li&gt; &lt;/li&gt; &lt;li&gt; get_product_picture/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; product_details/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; products &lt;/li&gt; &lt;li&gt; contact_us &lt;/li&gt; &lt;li&gt; add_to_cart/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; view_cart &lt;/li&gt; &lt;li&gt; delete_cart/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; login &lt;/li&gt; &lt;li&gt; signup &lt;/li&gt; &lt;li&gt; account_created &lt;/li&gt; &lt;li&gt; logout &lt;/li&gt; &lt;li&gt; checkout &lt;/li&gt; &lt;li&gt; payment &lt;/li&gt; &lt;li&gt; delete_account &lt;/li&gt; &lt;li&gt; brand_products/&amp;lt;str:brand&amp;gt; &lt;/li&gt; &lt;li&gt; category_products/&amp;lt;int:category_id&amp;gt; &lt;/li&gt; &lt;li&gt; test_cases &lt;/li&gt; &lt;li&gt; api_list &lt;/li&gt; &lt;li&gt; download_invoice/&amp;lt;int:overall_amount&amp;gt; &lt;/li&gt; &lt;li&gt; payment_done/&amp;lt;int:overall_amount&amp;gt; &lt;/li&gt; &lt;li&gt; video_tutorials &lt;/li&gt; &lt;li&gt; api/productsList &lt;/li&gt; &lt;li&gt; api/brandsList &lt;/li&gt; &lt;li&gt; api/searchProduct &lt;/li&gt; &lt;li&gt; api/verifyLogin &lt;/li&gt; &lt;li&gt; api/createAccount &lt;/li&gt; &lt;li&gt; api/deleteAccount &lt;/li&gt; &lt;li&gt; api/updateAccount &lt;/li&gt; &lt;li&gt; api/getUserDetailByEmail &lt;/li&gt; &lt;li&gt; &amp;lt;str:random_string&amp;gt; &lt;/li&gt; &lt;li&gt; ^static/(?P&amp;lt;path&amp;gt;.*)$ &lt;/li&gt; &lt;/ol&gt; &lt;p&gt; The current path, &lt;code&gt;api/productList&lt;/code&gt;, didn’t match any of these. &lt;/p&gt; &lt;/div&gt; &lt;div id="explanation"&gt; &lt;p&gt; You’re seeing this error because you have &lt;code&gt;DEBUG = True&lt;/code&gt; in your Django settings file. Change that to &lt;code&gt;False&lt;/code&gt;, and Django will display a standard 404 page. &lt;/p&gt; &lt;/div&gt; &lt;/body&gt; &lt;/html&gt;</t>
+  </si>
+  <si>
     <t>Column 7</t>
   </si>
   <si>
@@ -1178,16 +1193,46 @@
     <t>Response Code 200, “User exists!”</t>
   </si>
   <si>
+    <t>{ "responseCode": 200, "message": "User exists!" }</t>
+  </si>
+  <si>
     <t>TC_API09_003</t>
   </si>
   <si>
     <t>Verify DELETE with wrong endpoint returns 404</t>
   </si>
   <si>
+    <t>/api/verifyLoginXYZ</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt; &lt;html lang="en"&gt; &lt;head&gt; &lt;meta http-equiv="content-type" content="text/html; charset=utf-8"&gt; &lt;title&gt;Page not found at /api/verifyLoginXYZ&lt;/title&gt; &lt;meta name="robots" content="NONE,NOARCHIVE"&gt; &lt;style type="text/css"&gt; html * { padding: 0; margin: 0; } body * { padding: 10px 20px; } body * * { padding: 0; } body { font:small sans-serif; background:#eee; color:#000; } body&gt;div { border-bottom: 1px solid #ddd; } h1 { font-weight:normal; margin-bottom:.4em; } h1 span { font-size: 60%; color:#666; font-weight:normal; } table { border:none; border-collapse: collapse; width: 100%; } td, th { vertical-align:top; padding: 2px 3px; } th { width:12em; text-align:right; color:#666; padding-right:.5em; } #info { background:#f6f6f6; } #info ol { margin: 0.5em 4em; } #info ol li { font-family: monospace; } #summary { background: #ffc; } #explanation { background:#eee; border-bottom: 0px none; } pre.exception_value { font-family: sans-serif; color: #575757; font-size: 1.5em; margin: 10px 0 10px 0; } &lt;/style&gt; &lt;/head&gt; &lt;body&gt; &lt;div id="summary"&gt; &lt;h1&gt;Page not found &lt;span&gt;(404)&lt;/span&gt;&lt;/h1&gt; &lt;table class="meta"&gt; &lt;tr&gt; &lt;th&gt;Request Method:&lt;/th&gt; &lt;td&gt;DELETE&lt;/td&gt; &lt;/tr&gt; &lt;tr&gt; &lt;th&gt;Request URL:&lt;/th&gt; &lt;td&gt;https: //automationexercise.com/api/verifyLoginXYZ&lt;/td&gt; &lt;/tr&gt; &lt;/table&gt; &lt;/div&gt; &lt;div id="info"&gt; &lt;p&gt; Using the URLconf defined in &lt;code&gt;automation_exercise.urls&lt;/code&gt;, Django tried these URL patterns, in this order: &lt;/p&gt; &lt;ol&gt; &lt;li&gt; admin/ &lt;/li&gt; &lt;li&gt; &lt;/li&gt; &lt;li&gt; get_product_picture/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; product_details/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; products &lt;/li&gt; &lt;li&gt; contact_us &lt;/li&gt; &lt;li&gt; add_to_cart/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; view_cart &lt;/li&gt; &lt;li&gt; delete_cart/&amp;lt;int:product_id&amp;gt; &lt;/li&gt; &lt;li&gt; login &lt;/li&gt; &lt;li&gt; signup &lt;/li&gt; &lt;li&gt; account_created &lt;/li&gt; &lt;li&gt; logout &lt;/li&gt; &lt;li&gt; checkout &lt;/li&gt; &lt;li&gt; payment &lt;/li&gt; &lt;li&gt; delete_account &lt;/li&gt; &lt;li&gt; brand_products/&amp;lt;str:brand&amp;gt; &lt;/li&gt; &lt;li&gt; category_products/&amp;lt;int:category_id&amp;gt; &lt;/li&gt; &lt;li&gt; test_cases &lt;/li&gt; &lt;li&gt; api_list &lt;/li&gt; &lt;li&gt; download_invoice/&amp;lt;int:overall_amount&amp;gt; &lt;/li&gt; &lt;li&gt; payment_done/&amp;lt;int:overall_amount&amp;gt; &lt;/li&gt; &lt;li&gt; video_tutorials &lt;/li&gt; &lt;li&gt; api/productsList &lt;/li&gt; &lt;li&gt; api/brandsList &lt;/li&gt; &lt;li&gt; api/searchProduct &lt;/li&gt; &lt;li&gt; api/verifyLogin &lt;/li&gt; &lt;li&gt; api/createAccount &lt;/li&gt; &lt;li&gt; api/deleteAccount &lt;/li&gt; &lt;li&gt; api/updateAccount &lt;/li&gt; &lt;li&gt; api/getUserDetailByEmail &lt;/li&gt; &lt;li&gt; &amp;lt;str:random_string&amp;gt; &lt;/li&gt; &lt;li&gt; ^static/(?P&amp;lt;path&amp;gt;.*)$ &lt;/li&gt; &lt;/ol&gt; &lt;p&gt; The current path, &lt;code&gt;api/verifyLoginXYZ&lt;/code&gt;, didn’t match any of these. &lt;/p&gt; &lt;/div&gt; &lt;div id="explanation"&gt; &lt;p&gt; You’re seeing this error because you have &lt;code&gt;DEBUG = True&lt;/code&gt; in your Django settings file. Change that to &lt;code&gt;False&lt;/code&gt;, and Django will display a standard 404 page. &lt;/p&gt; &lt;/div&gt; &lt;/body&gt; &lt;/html&gt;</t>
+  </si>
+  <si>
     <t>TC_API6_001</t>
   </si>
   <si>
     <t>Verify Search without insert data</t>
+  </si>
+  <si>
+    <t>https://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>without pody</t>
+  </si>
+  <si>
+    <t>Message 400</t>
+  </si>
+  <si>
+    <t>ahmed kamal mohamed</t>
+  </si>
+  <si>
+    <t>TC_API6_002</t>
+  </si>
+  <si>
+    <t>Verify the search with another method (get insted of Post)</t>
   </si>
   <si>
     <r>
@@ -1199,33 +1244,6 @@
     </r>
   </si>
   <si>
-    <t>Post</t>
-  </si>
-  <si>
-    <t>without pody</t>
-  </si>
-  <si>
-    <t>Message 400</t>
-  </si>
-  <si>
-    <t>ahmed kamal mohamed</t>
-  </si>
-  <si>
-    <t>TC_API6_002</t>
-  </si>
-  <si>
-    <t>Verify the search with another method (get insted of Post)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://automationexercise.com/api/searchProduct</t>
-    </r>
-  </si>
-  <si>
     <t>get</t>
   </si>
   <si>
@@ -1241,9 +1259,6 @@
     <t>Verify that the response code is 400</t>
   </si>
   <si>
-    <t>https://automationexercise.com/api/searchProduct</t>
-  </si>
-  <si>
     <t>post</t>
   </si>
   <si>
@@ -1341,13 +1356,16 @@
   </si>
   <si>
     <t>response code 400 bad request</t>
+  </si>
+  <si>
+    <t>NotTested</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1372,6 +1390,11 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
@@ -1534,20 +1557,20 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -11682,9 +11705,11 @@
       <c r="F3" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>347</v>
+      </c>
       <c r="H3" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>31</v>
@@ -11704,7 +11729,7 @@
         <v>350</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>229</v>
+        <v>351</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>53</v>
@@ -11713,11 +11738,13 @@
         <v>345</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>352</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="H4" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>31</v>
@@ -11731,10 +11758,10 @@
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>229</v>
@@ -11746,11 +11773,13 @@
         <v>345</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>356</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>357</v>
+      </c>
       <c r="H5" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>31</v>
@@ -11792,10 +11821,10 @@
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>211</v>
@@ -11807,11 +11836,13 @@
         <v>345</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="G7" s="3"/>
       <c r="H7" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>31</v>
@@ -11825,10 +11856,10 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>211</v>
@@ -11840,11 +11871,13 @@
         <v>345</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>363</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>364</v>
+      </c>
       <c r="H8" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>31</v>
@@ -11858,13 +11891,13 @@
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>14</v>
@@ -11873,11 +11906,13 @@
         <v>345</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>368</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>369</v>
+      </c>
       <c r="H9" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>38</v>
@@ -11909,7 +11944,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>7</v>
@@ -11926,26 +11961,28 @@
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>345</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>374</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="H14" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>31</v>
@@ -11959,10 +11996,10 @@
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>13</v>
@@ -11971,14 +12008,16 @@
         <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>378</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>379</v>
+      </c>
       <c r="H15" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>38</v>
@@ -11992,26 +12031,28 @@
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>382</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>345</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>368</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>383</v>
+      </c>
       <c r="H16" s="6" t="s">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>38</v>
@@ -12172,140 +12213,140 @@
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="12" t="s">
-        <v>347</v>
+      <c r="H4" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>385</v>
+        <v>392</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>393</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="G5" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>347</v>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>391</v>
+        <v>398</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>386</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="F6" s="3">
         <v>400.0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>347</v>
+        <v>400</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>391</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>396</v>
+      <c r="F7" s="31" t="s">
+        <v>403</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>347</v>
+        <v>403</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8">
@@ -12351,233 +12392,233 @@
     </row>
     <row r="11" ht="22.5" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32" t="s">
-        <v>347</v>
+        <v>409</v>
+      </c>
+      <c r="G11" s="32"/>
+      <c r="H11" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32" t="s">
-        <v>347</v>
+        <v>412</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>400</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32" t="s">
-        <v>347</v>
+        <v>416</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32" t="s">
-        <v>347</v>
+        <v>420</v>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32" t="s">
-        <v>347</v>
+        <v>424</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32" t="s">
-        <v>347</v>
+      <c r="G16" s="32"/>
+      <c r="H16" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32" t="s">
-        <v>347</v>
+        <v>431</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -12873,7 +12914,7 @@
         <v>94</v>
       </c>
       <c r="C113" s="33" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D113" s="34" t="s">
         <v>14</v>
@@ -12886,13 +12927,13 @@
       </c>
       <c r="G113" s="35"/>
       <c r="H113" s="36" t="s">
-        <v>347</v>
+        <v>432</v>
       </c>
       <c r="I113" s="35" t="s">
         <v>31</v>
       </c>
       <c r="J113" s="37" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="K113" s="35"/>
     </row>

</xml_diff>